<commit_message>
Volunteers are now separated
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kathy.craven\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaderw\Desktop\JD\Dev\MyHometown\MHT Dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8C8F133D-C574-4610-A6DF-7E7F63417899}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B63834B-3325-43C8-A594-C736C7F82DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0606B945-0371-42CF-BA76-66F8ADCADBD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0606B945-0371-42CF-BA76-66F8ADCADBD9}"/>
   </bookViews>
   <sheets>
     <sheet name="missionaries-template (8)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
   <si>
     <t>State Position Options</t>
   </si>
@@ -280,9 +280,6 @@
     <t>Community Names</t>
   </si>
   <si>
-    <t>Remove Rows 1-18 Before Uploading</t>
-  </si>
-  <si>
     <t>Provost</t>
   </si>
   <si>
@@ -290,13 +287,22 @@
   </si>
   <si>
     <t>Community Technology Specialist</t>
+  </si>
+  <si>
+    <t>Remove Rows 1-20 Before Uploading</t>
+  </si>
+  <si>
+    <t>Community Executive Secratary</t>
+  </si>
+  <si>
+    <t>Save completed missionary roster as CSV File before uploading</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -443,6 +449,14 @@
     <font>
       <b/>
       <sz val="22"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -796,17 +810,23 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1254,7 +1274,7 @@
   <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,7 +1300,7 @@
     <col min="19" max="19" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -1303,12 +1323,12 @@
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4"/>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>78</v>
       </c>
       <c r="D2" s="4"/>
@@ -1326,12 +1346,12 @@
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>79</v>
       </c>
       <c r="D3" s="4"/>
@@ -1349,12 +1369,12 @@
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B4" s="4"/>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>71</v>
       </c>
       <c r="D4" s="4"/>
@@ -1367,17 +1387,17 @@
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="J4" s="4"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="4"/>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>80</v>
       </c>
       <c r="D5" s="4"/>
@@ -1390,18 +1410,18 @@
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="J5" s="4"/>
       <c r="K5" s="4"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="6" t="s">
-        <v>87</v>
+      <c r="C6" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
@@ -1409,17 +1429,17 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="4"/>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>72</v>
       </c>
       <c r="D7" s="4"/>
@@ -1428,17 +1448,17 @@
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="4"/>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>73</v>
       </c>
       <c r="D8" s="4"/>
@@ -1447,15 +1467,15 @@
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>74</v>
       </c>
       <c r="D9" s="4"/>
@@ -1464,23 +1484,23 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
-      <c r="M9" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="5"/>
-      <c r="R9" s="5"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M9" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+    </row>
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>75</v>
       </c>
       <c r="D10" s="4"/>
@@ -1489,21 +1509,21 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
-      <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="5"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>76</v>
       </c>
       <c r="D11" s="4"/>
@@ -1512,15 +1532,21 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J11" s="4"/>
       <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="6"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>77</v>
       </c>
       <c r="D12" s="4"/>
@@ -1528,14 +1554,22 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
+      <c r="I12" s="4" t="s">
+        <v>27</v>
+      </c>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>81</v>
       </c>
       <c r="D13" s="4"/>
@@ -1547,10 +1581,10 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>82</v>
       </c>
       <c r="D14" s="4"/>
@@ -1562,10 +1596,10 @@
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>55</v>
       </c>
       <c r="D15" s="4"/>
@@ -1576,11 +1610,20 @@
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="M15" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>83</v>
       </c>
       <c r="D16" s="4"/>
@@ -1591,11 +1634,18 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M16" s="8"/>
+      <c r="N16" s="8"/>
+      <c r="O16" s="8"/>
+      <c r="P16" s="8"/>
+      <c r="Q16" s="8"/>
+      <c r="R16" s="8"/>
+      <c r="S16" s="8"/>
+    </row>
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>84</v>
       </c>
       <c r="D17" s="4"/>
@@ -1606,11 +1656,17 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+    </row>
+    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D18" s="4"/>
@@ -1621,11 +1677,17 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>12</v>
       </c>
       <c r="D19" s="4"/>
@@ -1640,7 +1702,7 @@
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
@@ -1800,7 +1862,7 @@
         <v>6</v>
       </c>
       <c r="K23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="L23" s="1">
         <v>45337</v>
@@ -1825,8 +1887,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="M9:R10"/>
+  <mergeCells count="2">
+    <mergeCell ref="M9:R12"/>
+    <mergeCell ref="M15:S16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Bulk import is refined
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaderw\Desktop\JD\Dev\MyHometown\MHT Dashboard\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaderw\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B63834B-3325-43C8-A594-C736C7F82DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD327F74-16B6-45E5-B0E3-C39C1C53CCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{0606B945-0371-42CF-BA76-66F8ADCADBD9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0606B945-0371-42CF-BA76-66F8ADCADBD9}"/>
   </bookViews>
   <sheets>
     <sheet name="missionaries-template (8)" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="93">
   <si>
     <t>State Position Options</t>
   </si>
@@ -289,20 +289,23 @@
     <t>Community Technology Specialist</t>
   </si>
   <si>
-    <t>Remove Rows 1-20 Before Uploading</t>
-  </si>
-  <si>
     <t>Community Executive Secratary</t>
   </si>
   <si>
     <t>Save completed missionary roster as CSV File before uploading</t>
+  </si>
+  <si>
+    <t>Remove Rows 1-28 Before Uploading</t>
+  </si>
+  <si>
+    <t>Template Options</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -462,6 +465,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -650,7 +662,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -765,6 +777,86 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -810,24 +902,61 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -889,69 +1018,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Right Brace 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5415D275-2209-2543-D2D9-39A166C81860}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="10525125" y="19050"/>
-          <a:ext cx="800100" cy="3781425"/>
-        </a:xfrm>
-        <a:prstGeom prst="rightBrace">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="en-US" sz="1100"/>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1271,10 +1337,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76F98BD-6FEE-4080-A6B7-006F13567997}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:X31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M18" sqref="M18"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1300,598 +1366,768 @@
     <col min="19" max="19" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="23"/>
+    </row>
+    <row r="2" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="8"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
+      <c r="D3" s="20"/>
+      <c r="E3" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="2" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="2" t="s">
+      <c r="H3" s="20"/>
+      <c r="I3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="2" t="s">
+      <c r="J3" s="20"/>
+      <c r="K3" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="L3" s="20"/>
+      <c r="M3" s="25"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4" t="s">
+      <c r="H4" s="6"/>
+      <c r="I4" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
+      <c r="J4" s="6"/>
+      <c r="K4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="L4" s="6"/>
+      <c r="M4" s="8"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="5" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4" t="s">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4" t="s">
+      <c r="H5" s="6"/>
+      <c r="I5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="L5" s="6"/>
+      <c r="M5" s="8"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="5" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="F6" s="6"/>
+      <c r="G6" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4" t="s">
+      <c r="H6" s="6"/>
+      <c r="I6" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4" t="s">
+      <c r="J6" s="6"/>
+      <c r="K6" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="L6" s="6"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L7" s="6"/>
+      <c r="M7" s="8"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A8" s="5"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="L8" s="6"/>
+      <c r="M8" s="8"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="6"/>
+      <c r="E9" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="L9" s="6"/>
+      <c r="M9" s="8"/>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="8"/>
+    </row>
+    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="L11" s="6"/>
+      <c r="M11" s="8"/>
+    </row>
+    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L12" s="6"/>
+      <c r="M12" s="8"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="L13" s="6"/>
+      <c r="M13" s="8"/>
+      <c r="P13" s="3"/>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="6"/>
+      <c r="M14" s="8"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="8"/>
+      <c r="P15" s="3"/>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="3"/>
+      <c r="S15" s="3"/>
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="8"/>
+    </row>
+    <row r="17" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="8"/>
+    </row>
+    <row r="18" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="8"/>
+    </row>
+    <row r="19" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="8"/>
+      <c r="O19" s="2"/>
+      <c r="P19" s="2"/>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="2"/>
+      <c r="S19" s="2"/>
+      <c r="T19" s="2"/>
+    </row>
+    <row r="20" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5"/>
+      <c r="B20" s="6"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="8"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+    </row>
+    <row r="21" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
+      <c r="M21" s="8"/>
+      <c r="R21" s="4"/>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4"/>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="4"/>
+      <c r="X21" s="4"/>
+    </row>
+    <row r="22" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
+      <c r="M22" s="8"/>
+      <c r="R22" s="4"/>
+      <c r="S22" s="4"/>
+      <c r="T22" s="4"/>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="4"/>
+      <c r="X22" s="4"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5"/>
+      <c r="B23" s="6"/>
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="8"/>
+    </row>
+    <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="B24" s="10"/>
+      <c r="C24" s="10"/>
+      <c r="D24" s="10"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="10"/>
+      <c r="J24" s="10"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="10"/>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="10"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="10"/>
+      <c r="J25" s="10"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="B26" s="13"/>
+      <c r="C26" s="13"/>
+      <c r="D26" s="13"/>
+      <c r="E26" s="13"/>
+      <c r="F26" s="13"/>
+      <c r="G26" s="13"/>
+      <c r="H26" s="13"/>
+      <c r="I26" s="13"/>
+      <c r="J26" s="13"/>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="12"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="13"/>
+      <c r="D27" s="13"/>
+      <c r="E27" s="13"/>
+      <c r="F27" s="13"/>
+      <c r="G27" s="13"/>
+      <c r="H27" s="13"/>
+      <c r="I27" s="13"/>
+      <c r="J27" s="13"/>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="14"/>
+    </row>
+    <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="15"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="17"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="16"/>
+      <c r="H28" s="16"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="16"/>
+      <c r="K28" s="16"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="18"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F29" t="s">
+        <v>33</v>
+      </c>
+      <c r="G29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" t="s">
+        <v>36</v>
+      </c>
+      <c r="J29" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" t="s">
+        <v>38</v>
+      </c>
+      <c r="L29" t="s">
+        <v>39</v>
+      </c>
+      <c r="M29" t="s">
+        <v>40</v>
+      </c>
+      <c r="N29" t="s">
+        <v>41</v>
+      </c>
+      <c r="O29" t="s">
+        <v>42</v>
+      </c>
+      <c r="P29" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>44</v>
+      </c>
+      <c r="R29" t="s">
+        <v>45</v>
+      </c>
+      <c r="S29" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>47</v>
+      </c>
+      <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="s">
+        <v>51</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" t="s">
+        <v>53</v>
+      </c>
+      <c r="H30" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" t="s">
+        <v>55</v>
+      </c>
+      <c r="J30" t="s">
+        <v>27</v>
+      </c>
+      <c r="K30" t="s">
+        <v>68</v>
+      </c>
+      <c r="L30" s="1">
+        <v>45292</v>
+      </c>
+      <c r="M30" s="1">
+        <v>45657</v>
+      </c>
+      <c r="N30" t="s">
+        <v>56</v>
+      </c>
+      <c r="O30" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="M9" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="N9" s="6"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="6"/>
-      <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6"/>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J12" s="4"/>
-      <c r="K12" s="4"/>
-      <c r="M12" s="6"/>
-      <c r="N12" s="6"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="6"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
-      <c r="M15" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="P15" s="8"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-      <c r="C16" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="4"/>
-      <c r="I16" s="4"/>
-      <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="8"/>
-      <c r="P16" s="8"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="8"/>
-      <c r="S16" s="8"/>
-    </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="M17" s="7"/>
-      <c r="N17" s="7"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="7"/>
-      <c r="Q17" s="7"/>
-      <c r="R17" s="7"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
-      <c r="B18" s="4"/>
-      <c r="C18" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="M18" s="7"/>
-      <c r="N18" s="7"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="7"/>
-      <c r="Q18" s="7"/>
-      <c r="R18" s="7"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="4"/>
-      <c r="B20" s="4"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" t="s">
-        <v>30</v>
-      </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F21" t="s">
-        <v>33</v>
-      </c>
-      <c r="G21" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" t="s">
-        <v>35</v>
-      </c>
-      <c r="I21" t="s">
-        <v>36</v>
-      </c>
-      <c r="J21" t="s">
-        <v>37</v>
-      </c>
-      <c r="K21" t="s">
-        <v>38</v>
-      </c>
-      <c r="L21" t="s">
-        <v>39</v>
-      </c>
-      <c r="M21" t="s">
-        <v>40</v>
-      </c>
-      <c r="N21" t="s">
-        <v>41</v>
-      </c>
-      <c r="O21" t="s">
-        <v>42</v>
-      </c>
-      <c r="P21" t="s">
+      <c r="P30" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q30">
+        <v>84101</v>
+      </c>
+      <c r="R30" t="s">
+        <v>58</v>
+      </c>
+      <c r="S30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" t="s">
+        <v>63</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+      <c r="F31" t="s">
+        <v>65</v>
+      </c>
+      <c r="G31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
         <v>43</v>
       </c>
-      <c r="Q21" t="s">
-        <v>44</v>
-      </c>
-      <c r="R21" t="s">
-        <v>45</v>
-      </c>
-      <c r="S21" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
-      <c r="D22" t="s">
-        <v>50</v>
-      </c>
-      <c r="E22" t="s">
-        <v>51</v>
-      </c>
-      <c r="F22" t="s">
-        <v>52</v>
-      </c>
-      <c r="G22" t="s">
-        <v>53</v>
-      </c>
-      <c r="H22" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" t="s">
-        <v>55</v>
-      </c>
-      <c r="J22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" t="s">
-        <v>68</v>
-      </c>
-      <c r="L22" s="1">
-        <v>45292</v>
-      </c>
-      <c r="M22" s="1">
-        <v>45657</v>
-      </c>
-      <c r="N22" t="s">
-        <v>56</v>
-      </c>
-      <c r="O22" t="s">
-        <v>10</v>
-      </c>
-      <c r="P22" t="s">
+      <c r="I31" t="s">
+        <v>67</v>
+      </c>
+      <c r="J31" t="s">
+        <v>6</v>
+      </c>
+      <c r="K31" t="s">
+        <v>87</v>
+      </c>
+      <c r="L31" s="1">
+        <v>45337</v>
+      </c>
+      <c r="M31" s="1">
+        <v>45702</v>
+      </c>
+      <c r="N31" t="s">
+        <v>69</v>
+      </c>
+      <c r="O31" t="s">
+        <v>7</v>
+      </c>
+      <c r="P31" t="s">
         <v>57</v>
       </c>
-      <c r="Q22">
-        <v>84101</v>
-      </c>
-      <c r="R22" t="s">
-        <v>58</v>
-      </c>
-      <c r="S22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23" t="s">
-        <v>61</v>
-      </c>
-      <c r="C23" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E23" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" t="s">
-        <v>65</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
-      </c>
-      <c r="H23" t="s">
-        <v>43</v>
-      </c>
-      <c r="I23" t="s">
-        <v>67</v>
-      </c>
-      <c r="J23" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" t="s">
-        <v>87</v>
-      </c>
-      <c r="L23" s="1">
-        <v>45337</v>
-      </c>
-      <c r="M23" s="1">
-        <v>45702</v>
-      </c>
-      <c r="N23" t="s">
-        <v>69</v>
-      </c>
-      <c r="O23" t="s">
-        <v>7</v>
-      </c>
-      <c r="P23" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q23">
+      <c r="Q31">
         <v>84302</v>
       </c>
-      <c r="S23" t="s">
+      <c r="S31" t="s">
         <v>70</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="M9:R12"/>
-    <mergeCell ref="M15:S16"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A24:M25"/>
+    <mergeCell ref="A26:M27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Community Executive Secretary to Dropdown
</commit_message>
<xml_diff>
--- a/public/Template.xlsx
+++ b/public/Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaderw\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaderw\Desktop\JD\Dev\MyHometown\MHT Dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DD327F74-16B6-45E5-B0E3-C39C1C53CCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F646A6-1317-4587-AFF6-A2B319117231}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0606B945-0371-42CF-BA76-66F8ADCADBD9}"/>
+    <workbookView xWindow="120" yWindow="30" windowWidth="19770" windowHeight="10770" xr2:uid="{0606B945-0371-42CF-BA76-66F8ADCADBD9}"/>
   </bookViews>
   <sheets>
     <sheet name="missionaries-template (8)" sheetId="1" r:id="rId1"/>
@@ -289,9 +289,6 @@
     <t>Community Technology Specialist</t>
   </si>
   <si>
-    <t>Community Executive Secratary</t>
-  </si>
-  <si>
     <t>Save completed missionary roster as CSV File before uploading</t>
   </si>
   <si>
@@ -299,6 +296,9 @@
   </si>
   <si>
     <t>Template Options</t>
+  </si>
+  <si>
+    <t>Community Executive Secretary</t>
   </si>
 </sst>
 </file>
@@ -915,37 +915,21 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -955,8 +939,24 @@
     <xf numFmtId="0" fontId="21" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="13" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1339,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A76F98BD-6FEE-4080-A6B7-006F13567997}">
   <dimension ref="A1:X31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1367,21 +1367,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
-      <c r="M1" s="23"/>
+      <c r="A1" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="19"/>
     </row>
     <row r="2" spans="1:21" ht="10.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
@@ -1399,31 +1399,31 @@
       <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B3" s="19"/>
-      <c r="C3" s="19" t="s">
+      <c r="B3" s="13"/>
+      <c r="C3" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="19" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="20"/>
-      <c r="G3" s="19" t="s">
+      <c r="F3" s="14"/>
+      <c r="G3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="19" t="s">
+      <c r="H3" s="14"/>
+      <c r="I3" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="19" t="s">
+      <c r="J3" s="14"/>
+      <c r="K3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="20"/>
-      <c r="M3" s="25"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="16"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="8"/>
@@ -1870,83 +1870,83 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B24" s="10"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="11"/>
+      <c r="A24" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="22"/>
     </row>
     <row r="25" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="11"/>
+      <c r="A25" s="20"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="22"/>
     </row>
     <row r="26" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B26" s="13"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="13"/>
-      <c r="E26" s="13"/>
-      <c r="F26" s="13"/>
-      <c r="G26" s="13"/>
-      <c r="H26" s="13"/>
-      <c r="I26" s="13"/>
-      <c r="J26" s="13"/>
-      <c r="K26" s="13"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="14"/>
+      <c r="A26" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="24"/>
+      <c r="J26" s="24"/>
+      <c r="K26" s="24"/>
+      <c r="L26" s="24"/>
+      <c r="M26" s="25"/>
     </row>
     <row r="27" spans="1:24" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="12"/>
-      <c r="B27" s="13"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="13"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
-      <c r="I27" s="13"/>
-      <c r="J27" s="13"/>
-      <c r="K27" s="13"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="14"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
+      <c r="F27" s="24"/>
+      <c r="G27" s="24"/>
+      <c r="H27" s="24"/>
+      <c r="I27" s="24"/>
+      <c r="J27" s="24"/>
+      <c r="K27" s="24"/>
+      <c r="L27" s="24"/>
+      <c r="M27" s="25"/>
     </row>
     <row r="28" spans="1:24" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="16"/>
-      <c r="G28" s="16"/>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
-      <c r="J28" s="16"/>
-      <c r="K28" s="16"/>
-      <c r="L28" s="16"/>
-      <c r="M28" s="18"/>
+      <c r="A28" s="9"/>
+      <c r="B28" s="10"/>
+      <c r="C28" s="10"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="10"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="12"/>
     </row>
     <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" t="s">

</xml_diff>